<commit_message>
Wrong file be uploaded
</commit_message>
<xml_diff>
--- a/abapol.xlsx
+++ b/abapol.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{648B2A07-6EA7-4134-B787-143EA9B59341}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{530E889E-37B3-421D-A213-405981E9247E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4950" yWindow="2685" windowWidth="22485" windowHeight="11295"/>
   </bookViews>
@@ -3938,7 +3938,7 @@
   <dimension ref="A1:H1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3994,8 +3994,8 @@
         <v>2</v>
       </c>
       <c r="H2" s="2">
-        <f>COUNTIFS(D:D,"&lt;4",E:E,"=5",F:F,"=5")</f>
-        <v>17</v>
+        <f>COUNTIFS(D:D,"&lt;4",D:D,"&gt;0",E:E,"=5",F:F,"=5")</f>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>